<commit_message>
Se agrega segundo cv
</commit_message>
<xml_diff>
--- a/CV_Díaz_Juan/info_cv.xlsx
+++ b/CV_Díaz_Juan/info_cv.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Documents\CV\CV_Díaz_Juan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293AA3C4-6294-4A23-BC5C-A9B36F10A214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E753815-9BEE-4836-B853-94771DB65992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{34DB0F05-D7C4-422F-BAAA-B0A980F53D90}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{34DB0F05-D7C4-422F-BAAA-B0A980F53D90}"/>
   </bookViews>
   <sheets>
     <sheet name="Formación academica" sheetId="1" r:id="rId1"/>
     <sheet name="Experiencia laboral" sheetId="3" r:id="rId2"/>
     <sheet name="Formación complementaria" sheetId="2" r:id="rId3"/>
+    <sheet name="Publicaciones" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Grado</t>
   </si>
@@ -119,16 +120,33 @@
   </si>
   <si>
     <t>Me desenvolví principalmente en investigación, evaluación educativa y pricometría</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ponencia - "Estimación de la probabilidad de rezago en las asignaturas del plan de estudios de Psicología en la UNAM: Modelo de Rash"</t>
+  </si>
+  <si>
+    <t>VII Simposio Internacional de Psicología</t>
+  </si>
+  <si>
+    <t>Referencia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -151,16 +169,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -618,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B104E4-52D1-41B1-BF8F-7BF1CF5816BB}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,4 +713,50 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196DEECC-116E-43F5-869C-3096EF2D6618}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>2021</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se agregó link de Linkedin
</commit_message>
<xml_diff>
--- a/CV_Díaz_Juan/info_cv.xlsx
+++ b/CV_Díaz_Juan/info_cv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Documents\CV\CV_Díaz_Juan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC5E610-A880-4C2F-AE65-A92559E8F1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844ED862-1038-476D-81AB-FF41CAB71DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{34DB0F05-D7C4-422F-BAAA-B0A980F53D90}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{34DB0F05-D7C4-422F-BAAA-B0A980F53D90}"/>
   </bookViews>
   <sheets>
     <sheet name="Formación academica" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
   <si>
     <t>Grado</t>
   </si>
@@ -58,9 +57,6 @@
     <t>Licenciatura en Psicología</t>
   </si>
   <si>
-    <t>2016-2022</t>
-  </si>
-  <si>
     <t>Facultad de Psicología, UNAM</t>
   </si>
   <si>
@@ -118,9 +114,6 @@
     <t>Ponencia - "Estimación de la probabilidad de rezago en las asignaturas del plan de estudios de Psicología en la UNAM: Modelo de Rash"</t>
   </si>
   <si>
-    <t>Mi formación profesional está enfocada en investigación, evaluación educativa y psicometría.</t>
-  </si>
-  <si>
     <t>UNAM, Laboratorio de estudios sobre desarrollo numérico</t>
   </si>
   <si>
@@ -146,6 +139,48 @@
   </si>
   <si>
     <t>Curso - "Búsqueda de información y biblioteca digital"</t>
+  </si>
+  <si>
+    <t>2021 - 2022</t>
+  </si>
+  <si>
+    <t>Innova Schools</t>
+  </si>
+  <si>
+    <t>Coordinador de desarrollo de reactivos</t>
+  </si>
+  <si>
+    <t>Asistente de proyecto</t>
+  </si>
+  <si>
+    <t>2020 - 2021</t>
+  </si>
+  <si>
+    <t>Departamento de Matemática Educativa del Cinvestav</t>
+  </si>
+  <si>
+    <t>Generación y redacción de reactivos para evaluaciones en educación básica en las áreas de comunicación, matemáticas y ciencias</t>
+  </si>
+  <si>
+    <t>https://repository.ucatolica.edu.co/server/api/core/bitstreams/997221e5-af67-42b4-adea-9d67a6c2cd9f/content</t>
+  </si>
+  <si>
+    <t>Proyecto de titulación - "Relación entre el desempeño en tareas de discriminación numérica, temporal y espacial en diferentes grupos de edad"</t>
+  </si>
+  <si>
+    <t>Titulado el 18 de noviembre del 2022</t>
+  </si>
+  <si>
+    <t>Supervisor</t>
+  </si>
+  <si>
+    <t>2017-2022</t>
+  </si>
+  <si>
+    <t>UNAM, Programa de iniciación tempra a la investigación (PiTIP)</t>
+  </si>
+  <si>
+    <t>Manejo de grupos</t>
   </si>
 </sst>
 </file>
@@ -190,7 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -198,6 +233,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -516,13 +552,13 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="88.5703125" bestFit="1" customWidth="1"/>
@@ -532,7 +568,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -549,17 +585,17 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -570,10 +606,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F839D54-E766-4C3B-8340-6749AD15D5EB}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,7 +620,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -601,57 +637,109 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>2021</v>
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>2021</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -659,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B104E4-52D1-41B1-BF8F-7BF1CF5816BB}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +759,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -688,72 +776,72 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>2015</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>2019</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>2019</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>2019</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>2022</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -766,7 +854,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +865,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -786,52 +874,55 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>2016</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>2019</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>2021</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>2022</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>